<commit_message>
Updated UCID and Increment Matrix
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/Increment Matrix.xlsx
+++ b/Iteration 2 docs/Increment Matrix.xlsx
@@ -5,22 +5,36 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Documents\Academic\2020 Fall\CSE 5324 SE-1\Iteration 2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Downloads\CarRental\Iteration 2 docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51E95584-D615-4325-9BAE-A11796F16C2D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473A2B75-4926-4B8D-B1DB-BBE18CEF498F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inc Matrix" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Inc Matrix'!$A$1:$F$22</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
   <si>
     <t>Use Case Name</t>
   </si>
@@ -100,12 +114,6 @@
     <t>UC 21</t>
   </si>
   <si>
-    <t>UC 22</t>
-  </si>
-  <si>
-    <t>UC 23</t>
-  </si>
-  <si>
     <t>View Profile</t>
   </si>
   <si>
@@ -139,15 +147,6 @@
     <t>View User</t>
   </si>
   <si>
-    <t>Edit User Profile</t>
-  </si>
-  <si>
-    <t>Update User Role</t>
-  </si>
-  <si>
-    <t>Revoke Renter</t>
-  </si>
-  <si>
     <t>View Reservation Calendar</t>
   </si>
   <si>
@@ -170,13 +169,93 @@
   </si>
   <si>
     <t xml:space="preserve">Iteration 3* </t>
+  </si>
+  <si>
+    <t>Omkar</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>InProgress</t>
+  </si>
+  <si>
+    <t>Not Started</t>
+  </si>
+  <si>
+    <t>Search Vehicles ---&gt; Select Vehicle --&gt; Reserve Rental</t>
+  </si>
+  <si>
+    <t>View Reservation Calendar --&gt; View Rental Details --&gt; Delete Reservation</t>
+  </si>
+  <si>
+    <t>View Available Cars, Search for Car --&gt; View Selected Car</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">View Rental History --&gt; View Reservation Summary --&gt; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>{</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Update Rental Details, Cancel Rental Reservation</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="14"/>
+        <color rgb="FF92D050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>}</t>
+    </r>
+  </si>
+  <si>
+    <t>Function path</t>
+  </si>
+  <si>
+    <t>Assigned to</t>
+  </si>
+  <si>
+    <t>Modify User Profile</t>
+  </si>
+  <si>
+    <t>Gaurav</t>
+  </si>
+  <si>
+    <t>Neel</t>
+  </si>
+  <si>
+    <t>Jeevesh</t>
+  </si>
+  <si>
+    <t>Search All Users ---&gt; View User --&gt; { Modify User Profile }</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -319,13 +398,53 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -513,24 +632,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -669,6 +794,56 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -714,26 +889,98 @@
     <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -781,6 +1028,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1113,309 +1365,395 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" customWidth="1"/>
-    <col min="2" max="2" width="40" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="75.21875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.77734375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="10"/>
+      <c r="D2" s="5">
+        <v>1</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="4"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="10"/>
+      <c r="D3" s="5">
+        <v>1</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="10"/>
+      <c r="D4" s="5">
+        <v>1</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="4"/>
+      <c r="G4" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="10"/>
+      <c r="D5" s="5">
+        <v>1</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="4"/>
+      <c r="G5" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="10"/>
+      <c r="D6" s="5">
+        <v>1</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="20" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="D7" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="20"/>
+      <c r="D8" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F9" s="4"/>
+    </row>
+    <row r="10" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>52</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4">
         <v>1</v>
       </c>
-      <c r="D2" s="1"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1">
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C12" s="29"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
         <v>1</v>
       </c>
-      <c r="D3" s="1"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1">
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C13" s="30"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C5" s="1">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="21"/>
+      <c r="D15" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="21"/>
+      <c r="D16" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="4">
         <v>1</v>
       </c>
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C6" s="1">
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="26"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="4">
         <v>1</v>
       </c>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="1">
+      <c r="G18" s="13"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="4"/>
+      <c r="F19" s="4">
         <v>1</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="1">
-        <v>1</v>
-      </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1">
-        <v>1</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1</v>
-      </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="1">
-        <v>1</v>
-      </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C16" s="1">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B17" s="6" t="s">
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="6" t="s">
+      <c r="C20" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="4"/>
+      <c r="G20" s="15"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A19" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" s="4" t="s">
+      <c r="C21" s="23"/>
+      <c r="D21" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" s="19"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="C20" s="1">
-        <v>1</v>
-      </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1</v>
-      </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B23" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1">
-        <v>1</v>
-      </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="1">
-        <v>1</v>
-      </c>
-      <c r="D24" s="1"/>
+      <c r="C22" s="24"/>
+      <c r="D22" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E22" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" s="4"/>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="C10:C13"/>
+  </mergeCells>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Added Columns 'EUC' and 'UIP' in Increment Matrix.xlsx.
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/Increment Matrix.xlsx
+++ b/Iteration 2 docs/Increment Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Downloads\CarRental\Iteration 2 docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS 2020\Semester 3\CSE 5324 - SE - 1\ArlingtonAuto\Iteration 2 docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473A2B75-4926-4B8D-B1DB-BBE18CEF498F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A58963-8D0F-4A1C-9290-6DD5ED1D688E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inc Matrix" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
   <si>
     <t>Use Case Name</t>
   </si>
@@ -249,6 +249,15 @@
   </si>
   <si>
     <t>Search All Users ---&gt; View User --&gt; { Modify User Profile }</t>
+  </si>
+  <si>
+    <t>EUC</t>
+  </si>
+  <si>
+    <t>UIP</t>
+  </si>
+  <si>
+    <t>Done</t>
   </si>
 </sst>
 </file>
@@ -1365,25 +1374,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.21875" style="16" customWidth="1"/>
-    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.77734375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.21875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="1"/>
+    <col min="3" max="3" width="75.28515625" style="16" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1402,8 +1412,14 @@
       <c r="F1" s="3" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1418,8 +1434,12 @@
         <v>45</v>
       </c>
       <c r="F2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H2" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="4"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1437,8 +1457,12 @@
       <c r="G3" s="5" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H3" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1456,8 +1480,12 @@
       <c r="G4" s="9" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1475,8 +1503,12 @@
       <c r="G5" s="7" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H5" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1491,8 +1523,12 @@
         <v>45</v>
       </c>
       <c r="F6" s="6"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1509,8 +1545,12 @@
         <v>56</v>
       </c>
       <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H7" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1525,8 +1565,12 @@
         <v>56</v>
       </c>
       <c r="F8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H8" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -1541,8 +1585,12 @@
         <v>56</v>
       </c>
       <c r="F9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1557,8 +1605,10 @@
       <c r="F10" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1571,8 +1621,10 @@
       <c r="F11" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -1585,8 +1637,10 @@
       <c r="F12" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1599,8 +1653,10 @@
       <c r="F13" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -1617,8 +1673,12 @@
         <v>57</v>
       </c>
       <c r="F14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -1633,8 +1693,12 @@
         <v>57</v>
       </c>
       <c r="F15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H15" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -1649,8 +1713,12 @@
         <v>57</v>
       </c>
       <c r="F16" s="4"/>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1665,8 +1733,10 @@
       <c r="F17" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1680,8 +1750,10 @@
         <v>1</v>
       </c>
       <c r="G18" s="13"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1694,8 +1766,10 @@
       <c r="F19" s="4">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
@@ -1713,8 +1787,12 @@
       </c>
       <c r="F20" s="4"/>
       <c r="G20" s="15"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H20" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>24</v>
       </c>
@@ -1729,8 +1807,12 @@
         <v>58</v>
       </c>
       <c r="F21" s="19"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="H21" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>25</v>
       </c>
@@ -1745,6 +1827,10 @@
         <v>58</v>
       </c>
       <c r="F22" s="4"/>
+      <c r="H22" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="I22" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Updated the Column EUC in EUC_UIP.docx
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/Increment Matrix.xlsx
+++ b/Iteration 2 docs/Increment Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS 2020\Semester 3\CSE 5324 - SE - 1\ArlingtonAuto\Iteration 2 docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A58963-8D0F-4A1C-9290-6DD5ED1D688E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F731B295-B4A8-4098-8DCD-83D28103CB7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="64">
   <si>
     <t>Use Case Name</t>
   </si>
@@ -258,6 +258,9 @@
   </si>
   <si>
     <t>Done</t>
+  </si>
+  <si>
+    <t>Double Check</t>
   </si>
 </sst>
 </file>
@@ -1377,7 +1380,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1389,7 +1392,7 @@
     <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
     <col min="6" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
@@ -1586,7 +1589,7 @@
       </c>
       <c r="F9" s="4"/>
       <c r="H9" s="4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="I9" s="4"/>
     </row>
@@ -1674,7 +1677,7 @@
       </c>
       <c r="F14" s="4"/>
       <c r="H14" s="4" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="I14" s="4"/>
     </row>
@@ -1694,7 +1697,7 @@
       </c>
       <c r="F15" s="4"/>
       <c r="H15" s="4" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="I15" s="4"/>
     </row>
@@ -1714,7 +1717,7 @@
       </c>
       <c r="F16" s="4"/>
       <c r="H16" s="4" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="I16" s="4"/>
     </row>
@@ -1788,7 +1791,7 @@
       <c r="F20" s="4"/>
       <c r="G20" s="15"/>
       <c r="H20" s="4" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="I20" s="4"/>
     </row>
@@ -1808,7 +1811,7 @@
       </c>
       <c r="F21" s="19"/>
       <c r="H21" s="4" t="s">
-        <v>48</v>
+        <v>62</v>
       </c>
       <c r="I21" s="4"/>
     </row>
@@ -1828,7 +1831,7 @@
       </c>
       <c r="F22" s="4"/>
       <c r="H22" s="4" t="s">
-        <v>48</v>
+        <v>63</v>
       </c>
       <c r="I22" s="4"/>
     </row>

</xml_diff>

<commit_message>
Added revoke functionality for search users.
</commit_message>
<xml_diff>
--- a/Iteration 2 docs/Increment Matrix.xlsx
+++ b/Iteration 2 docs/Increment Matrix.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MS 2020\Semester 3\CSE 5324 - SE - 1\ArlingtonAuto\Iteration 2 docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gaura\Downloads\CarRental\Iteration 2 docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F731B295-B4A8-4098-8DCD-83D28103CB7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5C3901-01DA-4950-A284-C69C0718F096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inc Matrix" sheetId="1" r:id="rId1"/>
@@ -1380,23 +1380,23 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="11.109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="75.28515625" style="16" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="75.33203125" style="16" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="12.6640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.33203125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
@@ -1422,7 +1422,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
@@ -1442,7 +1442,7 @@
       </c>
       <c r="I2" s="4"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1465,7 +1465,7 @@
       </c>
       <c r="I3" s="4"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1488,7 +1488,7 @@
       </c>
       <c r="I4" s="4"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="I5" s="4"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="I6" s="4"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -1541,8 +1541,8 @@
       <c r="C7" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>47</v>
+      <c r="D7" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>56</v>
@@ -1553,7 +1553,7 @@
       </c>
       <c r="I7" s="4"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -1561,8 +1561,8 @@
         <v>29</v>
       </c>
       <c r="C8" s="20"/>
-      <c r="D8" s="9" t="s">
-        <v>47</v>
+      <c r="D8" s="5" t="s">
+        <v>46</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>56</v>
@@ -1573,7 +1573,7 @@
       </c>
       <c r="I8" s="4"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -1593,7 +1593,7 @@
       </c>
       <c r="I9" s="4"/>
     </row>
-    <row r="10" spans="1:9" ht="16.149999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -1611,7 +1611,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -1627,7 +1627,7 @@
       <c r="H11" s="4"/>
       <c r="I11" s="4"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -1643,7 +1643,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -1659,7 +1659,7 @@
       <c r="H13" s="4"/>
       <c r="I13" s="4"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="I14" s="4"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -1701,7 +1701,7 @@
       </c>
       <c r="I15" s="4"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -1721,7 +1721,7 @@
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -1739,7 +1739,7 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>21</v>
       </c>
@@ -1756,7 +1756,7 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>22</v>
       </c>
@@ -1772,7 +1772,7 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>23</v>
       </c>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="I20" s="4"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>24</v>
       </c>
@@ -1815,7 +1815,7 @@
       </c>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>25</v>
       </c>

</xml_diff>